<commit_message>
Fix part list, cpl and JLC bom
</commit_message>
<xml_diff>
--- a/electronics/AKARI_Light/pcb/AKARI_Light_board_bom_JLCSMT.xlsx
+++ b/electronics/AKARI_Light/pcb/AKARI_Light_board_bom_JLCSMT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">C17414</t>
   </si>
   <si>
-    <t xml:space="preserve">https://jlcpcb.com/partdetail/18102-0805W8F1002T5E/C174142</t>
+    <t xml:space="preserve">https://jlcpcb.com/partdetail/18102-0805W8F1002T5E/C17414</t>
   </si>
   <si>
     <t xml:space="preserve">R0805 1k</t>
@@ -103,6 +103,21 @@
     <t xml:space="preserve">https://jlcpcb.com/partdetail/18201-0805W8F1001T5E/C17513</t>
   </si>
   <si>
+    <t xml:space="preserve">C0805 100nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0805KRX7R9BB104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C49678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://jlcpcb.com/partdetail/Yageo-CC0805KRX7R9BB104/C49678</t>
+  </si>
+  <si>
     <t xml:space="preserve">74HC126D</t>
   </si>
   <si>
@@ -131,105 +146,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://jlcpcb.com/partdetail/TexasInstruments-SN74AHC1G04DBVR/C7465</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIN Header 2X15 SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PZ254-2-15-S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3294473</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://jlcpcb.com/partdetail/Hctl-PZ254_2_15S/C3294473</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIN Header 2X13 L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM254-2-13-W-8.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2897433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://jlcpcb.com/partdetail/Hctl-PM254_2_13_W_85/C2897433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B4B-PH-K-S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B4B-PH-K-S-GW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C566011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://jlcpcb.com/partdetail/Jst_SalesAmerica-B4B_PH_K_SGW/C566011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH2.0-4A (Grove)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J4,J5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C403774</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://jlcpcb.com/partdetail/Seeed_Technology_co_Ltd-110990030/C403774</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-03-5035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C293315</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://jlcpcb.com/parts/componentSearch?searchTxt=22-03-5035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Box Header 2x5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS254P-2X5-L0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4749194</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://jlcpcb.com/partdetail/Dealon-DS254P_2X5L0/C4749194</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIN Header 2X1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PZ254V-11-02P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C492401</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://jlcpcb.com/partdetail/Xfcn-PZ254V_1102P/C492401</t>
   </si>
 </sst>
 </file>
@@ -341,7 +257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,6 +266,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,15 +286,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -458,283 +370,173 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="60.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="60.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+    <row r="3" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+    <row r="6" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>33</v>
-      </c>
+    <row r="7" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>38</v>
-      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>110990030</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>42</v>
-      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>22035035</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>46</v>
-      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>51</v>
-      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://jlcpcb.com/partdetail/18102-0805W8F1002T5E/C174142"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://jlcpcb.com/partdetail/18102-0805W8F1002T5E/C17414"/>
     <hyperlink ref="E3" r:id="rId2" display="https://jlcpcb.com/partdetail/18201-0805W8F1001T5E/C17513"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://jlcpcb.com/partdetail/TexasInstruments-SN74HC126DR/C7644"/>
-    <hyperlink ref="E5" r:id="rId4" display="https://jlcpcb.com/partdetail/TexasInstruments-SN74AHC1G04DBVR/C7465"/>
-    <hyperlink ref="E6" r:id="rId5" display="https://jlcpcb.com/partdetail/Hctl-PZ254_2_15S/C3294473"/>
-    <hyperlink ref="E7" r:id="rId6" display="https://jlcpcb.com/partdetail/Hctl-PM254_2_13_W_85/C2897433"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://jlcpcb.com/partdetail/Jst_SalesAmerica-B4B_PH_K_SGW/C566011"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://jlcpcb.com/partdetail/Seeed_Technology_co_Ltd-110990030/C403774"/>
-    <hyperlink ref="E10" r:id="rId9" display="https://jlcpcb.com/parts/componentSearch?searchTxt=22-03-5035"/>
-    <hyperlink ref="E11" r:id="rId10" display="https://jlcpcb.com/partdetail/Dealon-DS254P_2X5L0/C4749194"/>
-    <hyperlink ref="E12" r:id="rId11" display="https://jlcpcb.com/partdetail/Xfcn-PZ254V_1102P/C492401"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://jlcpcb.com/partdetail/Yageo-CC0805KRX7R9BB104/C49678"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://jlcpcb.com/partdetail/TexasInstruments-SN74HC126DR/C7644"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://jlcpcb.com/partdetail/TexasInstruments-SN74AHC1G04DBVR/C7465"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>